<commit_message>
Updated Manager Updated Task Dinamic Array
</commit_message>
<xml_diff>
--- a/Manager.xlsx
+++ b/Manager.xlsx
@@ -4,20 +4,21 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="24315" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="25920" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="ЗаданияПрограммисты" sheetId="1" r:id="rId1"/>
-    <sheet name="ЗаданияДизайнеры" sheetId="4" r:id="rId2"/>
-    <sheet name="Список участников" sheetId="3" r:id="rId3"/>
-    <sheet name="Статусы" sheetId="2" r:id="rId4"/>
+    <sheet name="Log" sheetId="5" r:id="rId2"/>
+    <sheet name="ЗаданияДизайнеры" sheetId="4" r:id="rId3"/>
+    <sheet name="Список участников" sheetId="3" r:id="rId4"/>
+    <sheet name="Статусы" sheetId="2" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="63">
   <si>
     <t>Дата задания</t>
   </si>
@@ -160,9 +161,6 @@
     <t>Насать деструктор для  GameMunu !Рекурентный</t>
   </si>
   <si>
-    <t>Настроить навигацию по меню через мышь</t>
-  </si>
-  <si>
     <t>Избавиться от нерационального использования памяти в Object</t>
   </si>
   <si>
@@ -176,6 +174,39 @@
   </si>
   <si>
     <t>Последний ping</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>Учимся проектировать классы</t>
+  </si>
+  <si>
+    <t>Level</t>
+  </si>
+  <si>
+    <t>Front</t>
+  </si>
+  <si>
+    <t>SandBox</t>
+  </si>
+  <si>
+    <t>Вычисление 3D преобразования координат</t>
+  </si>
+  <si>
+    <t>Заменить GameProcess::LoadFromFile на интерфейс</t>
+  </si>
+  <si>
+    <t>1-Проектирование</t>
+  </si>
+  <si>
+    <t>1-Отладка</t>
   </si>
 </sst>
 </file>
@@ -240,6 +271,18 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF0000FF"/>
+      <color rgb="FFFF0000"/>
+      <color rgb="FFC0FFC0"/>
+      <color rgb="FF800000"/>
+      <color rgb="FF000080"/>
+      <color rgb="FF80FF80"/>
+      <color rgb="FFFF8080"/>
+      <color rgb="FF00FF00"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -538,35 +581,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H29"/>
+  <dimension ref="A1:I42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G3" sqref="G3"/>
+      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.28515625" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="31.140625" customWidth="1"/>
-    <col min="6" max="6" width="24.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="31.140625" customWidth="1"/>
+    <col min="6" max="6" width="64.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="31.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B1" s="2">
         <f ca="1">NOW()</f>
-        <v>42064.733332175929</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+        <v>42065.84356134259</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -577,19 +620,22 @@
         <v>6</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F2" t="s">
         <v>2</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>3</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>42062.802245370367</v>
       </c>
@@ -597,149 +643,303 @@
         <v>42071</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>61</v>
       </c>
       <c r="D3" s="5">
-        <v>42064</v>
+        <v>42065</v>
       </c>
       <c r="E3" t="s">
+        <v>58</v>
+      </c>
+      <c r="F3" t="s">
         <v>37</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="G3" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>36</v>
       </c>
-      <c r="H3" s="2"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I3" s="2"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>42062.802245370367</v>
       </c>
       <c r="B4" s="3">
-        <v>42064.874988425923</v>
+        <v>42068.874988425923</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>62</v>
+      </c>
+      <c r="D4" s="5">
+        <v>42063</v>
       </c>
       <c r="E4" t="s">
-        <v>51</v>
-      </c>
-      <c r="F4" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F4" t="s">
         <v>50</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F5" s="1"/>
-      <c r="H5" s="2"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
+      <c r="H4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B5" s="3"/>
+      <c r="G5" s="1"/>
+      <c r="I5" s="2"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B6" s="3"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
+        <v>42065.833773379629</v>
+      </c>
       <c r="B7" s="3"/>
-      <c r="E7" t="s">
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <v>42065.833773379629</v>
+      </c>
       <c r="B8" s="3"/>
-      <c r="E8" t="s">
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
+        <v>42065.833773379629</v>
+      </c>
       <c r="B9" s="3"/>
-      <c r="E9" t="s">
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
+        <v>42065.833773379629</v>
+      </c>
       <c r="B10" s="3"/>
-      <c r="E10" t="s">
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="3">
+        <v>42065.833773379629</v>
+      </c>
       <c r="B11" s="3"/>
-      <c r="E11" t="s">
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="3">
+        <v>42065.833773379629</v>
+      </c>
       <c r="B12" s="3"/>
-      <c r="E12" t="s">
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B13" s="3"/>
-      <c r="E13" t="s">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="3">
+        <v>42065.833773379629</v>
+      </c>
+      <c r="B13" s="3">
+        <v>42071.666666666664</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="3">
+        <v>42065.833773379629</v>
+      </c>
+      <c r="B14" s="3">
+        <v>42071.666666666664</v>
+      </c>
+      <c r="E14">
+        <v>2</v>
+      </c>
+      <c r="F14" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="3">
+        <v>42065.833773379629</v>
+      </c>
+      <c r="B15" s="3">
+        <v>42071.666666666664</v>
+      </c>
+      <c r="E15">
+        <v>2</v>
+      </c>
+      <c r="F15" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="3">
+        <v>42065.833773379629</v>
+      </c>
+      <c r="B16" s="3">
+        <v>42071.666666666664</v>
+      </c>
+      <c r="E16">
+        <v>2</v>
+      </c>
+      <c r="F16" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="3">
+        <v>42065.833773379629</v>
+      </c>
+      <c r="B17" s="3">
+        <v>42071.666666666664</v>
+      </c>
+      <c r="E17">
+        <v>2</v>
+      </c>
+      <c r="F17" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B14" s="3"/>
-      <c r="E14" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B15" s="3"/>
-      <c r="E15" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B16" s="3"/>
-      <c r="E16" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B17" s="3"/>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B18" s="3"/>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B19" s="3"/>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B20" s="3"/>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B21" s="3"/>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B22" s="3"/>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B23" s="3"/>
     </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B24" s="3"/>
     </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B25" s="3"/>
     </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B26" s="3"/>
     </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B27" s="3"/>
     </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B28" s="3"/>
     </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B29" s="3"/>
     </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B30" s="3"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B31" s="3"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B32" s="3"/>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B33" s="3"/>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B34" s="3"/>
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B35" s="3"/>
+    </row>
+    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B36" s="3"/>
+    </row>
+    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B37" s="3"/>
+    </row>
+    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B38" s="3"/>
+    </row>
+    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B39" s="3"/>
+    </row>
+    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B40" s="3"/>
+    </row>
+    <row r="41" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B41" s="3"/>
+    </row>
+    <row r="42" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B42" s="3"/>
+    </row>
   </sheetData>
+  <conditionalFormatting sqref="B3:B12 B19:B1048576">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="num" val="$B$1"/>
+        <cfvo type="formula" val="$B$1+3"/>
+        <cfvo type="num" val="$B$1+7"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FFC0FFC0"/>
+        <color rgb="FF0000FF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B13:B18">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="num" val="$B$1"/>
+        <cfvo type="formula" val="$B$1+3"/>
+        <cfvo type="num" val="$B$1+7"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FFC0FFC0"/>
+        <color rgb="FF0000FF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="F3" r:id="rId1"/>
+    <hyperlink ref="G3" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
@@ -747,6 +947,49 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="52.85546875" customWidth="1"/>
+    <col min="4" max="4" width="45.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
+        <v>42065</v>
+      </c>
+      <c r="B2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G29"/>
   <sheetViews>
@@ -771,7 +1014,7 @@
       </c>
       <c r="B1" s="2">
         <f ca="1">NOW()</f>
-        <v>42064.733332175929</v>
+        <v>42065.84356134259</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -944,7 +1187,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D7"/>
   <sheetViews>
@@ -1070,7 +1313,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A4"/>
   <sheetViews>

</xml_diff>